<commit_message>
Fix conditional forecasts so wages feed into shortages
</commit_message>
<xml_diff>
--- a/Replication Package/Code and Data/(2) Regressions/Output Data Python (New Model Pre Covid)/eq_coefficients_new_model_pre_covid.xlsx
+++ b/Replication Package/Code and Data/(2) Regressions/Output Data Python (New Model Pre Covid)/eq_coefficients_new_model_pre_covid.xlsx
@@ -793,16 +793,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.042377674289254</v>
+        <v>4.162295600260551</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9282264015394623</v>
+        <v>1.107274434386906</v>
       </c>
       <c r="D2" t="n">
-        <v>3.277624585169604</v>
+        <v>3.759046060306811</v>
       </c>
       <c r="E2" t="n">
-        <v>0.001529904183642678</v>
+        <v>0.0003162805065090288</v>
       </c>
     </row>
     <row r="3">
@@ -812,16 +812,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03023121447526651</v>
+        <v>0.03023121447526297</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08811083674314929</v>
+        <v>0.08811083674314943</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3431043852573222</v>
+        <v>0.3431043852572815</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7323874358597391</v>
+        <v>0.7323874358597695</v>
       </c>
     </row>
     <row r="4">
@@ -831,16 +831,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.05788194520313884</v>
+        <v>0.05788194520314387</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08423686466846003</v>
+        <v>0.08423686466845988</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6871331860575647</v>
+        <v>0.6871331860576255</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4939143088192079</v>
+        <v>0.49391430881917</v>
       </c>
     </row>
     <row r="5">
@@ -850,16 +850,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2476551681717054</v>
+        <v>0.2476551681717035</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08264258064817082</v>
+        <v>0.0826425806481708</v>
       </c>
       <c r="D5" t="n">
-        <v>2.996701775638307</v>
+        <v>2.996701775638284</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00359849702274033</v>
+        <v>0.003598497022740576</v>
       </c>
     </row>
     <row r="6">
@@ -869,16 +869,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.257664536745656</v>
+        <v>0.2576645367456548</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08672326249814834</v>
+        <v>0.08672326249814835</v>
       </c>
       <c r="D6" t="n">
-        <v>2.971112125205823</v>
+        <v>2.971112125205809</v>
       </c>
       <c r="E6" t="n">
-        <v>0.003880380508392733</v>
+        <v>0.003880380508392888</v>
       </c>
     </row>
     <row r="7">
@@ -888,16 +888,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-1.652586040996542</v>
+        <v>-39.44707325299284</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7059806442107848</v>
+        <v>16.85169152862024</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.340837605886442</v>
+        <v>-2.340837605886478</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02163957395632586</v>
+        <v>0.02163957395632394</v>
       </c>
     </row>
     <row r="8">
@@ -907,16 +907,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.649509521087356</v>
+        <v>110.9833546447109</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9777229659947535</v>
+        <v>23.33815517252609</v>
       </c>
       <c r="D8" t="n">
-        <v>4.755446770504014</v>
+        <v>4.75544677050402</v>
       </c>
       <c r="E8" t="n">
-        <v>8.239817215566172e-06</v>
+        <v>8.239817215566001e-06</v>
       </c>
     </row>
     <row r="9">
@@ -926,16 +926,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1.583280842986272</v>
+        <v>-37.7927646996677</v>
       </c>
       <c r="C9" t="n">
-        <v>1.068481455294628</v>
+        <v>25.50455176969453</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.481804700625048</v>
+        <v>-1.481804700625027</v>
       </c>
       <c r="E9" t="n">
-        <v>0.142178998141526</v>
+        <v>0.1421789981415316</v>
       </c>
     </row>
     <row r="10">
@@ -945,16 +945,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-3.302471438892061</v>
+        <v>-78.82968240935431</v>
       </c>
       <c r="C10" t="n">
-        <v>1.072200740049378</v>
+        <v>25.59333074672177</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.080086886285839</v>
+        <v>-3.080086886285855</v>
       </c>
       <c r="E10" t="n">
-        <v>0.002806223942581848</v>
+        <v>0.002806223942581709</v>
       </c>
     </row>
     <row r="11">
@@ -964,16 +964,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.532988127822146</v>
+        <v>60.46218819983819</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7823151713858066</v>
+        <v>18.6737895074883</v>
       </c>
       <c r="D11" t="n">
-        <v>3.23781031030648</v>
+        <v>3.237810310306459</v>
       </c>
       <c r="E11" t="n">
-        <v>0.001732257796798422</v>
+        <v>0.00173225779679854</v>
       </c>
     </row>
     <row r="12">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.030439022059688</v>
+        <v>4.030439022059699</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7190811354684978</v>
+        <v>0.7190811354684982</v>
       </c>
       <c r="D12" t="n">
-        <v>5.604985061155532</v>
+        <v>5.604985061155546</v>
       </c>
       <c r="E12" t="n">
-        <v>2.652903284272096e-07</v>
+        <v>2.652903284271935e-07</v>
       </c>
     </row>
     <row r="13">
@@ -1002,16 +1002,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1.882362477267213</v>
+        <v>-1.882362477267233</v>
       </c>
       <c r="C13" t="n">
-        <v>1.034466677036621</v>
+        <v>1.034466677036626</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.819645348711969</v>
+        <v>-1.819645348711979</v>
       </c>
       <c r="E13" t="n">
-        <v>0.07241849061627494</v>
+        <v>0.07241849061627345</v>
       </c>
     </row>
     <row r="14">
@@ -1021,16 +1021,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0696325212998208</v>
+        <v>0.06963252129980541</v>
       </c>
       <c r="C14" t="n">
-        <v>1.014433579134346</v>
+        <v>1.014433579134348</v>
       </c>
       <c r="D14" t="n">
-        <v>0.06864177481116195</v>
+        <v>0.06864177481114662</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9454398639911386</v>
+        <v>0.9454398639911507</v>
       </c>
     </row>
     <row r="15">
@@ -1040,16 +1040,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.9068918658411471</v>
+        <v>-0.9068918658410942</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9822652333657452</v>
+        <v>0.982265233365745</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.9232657687920703</v>
+        <v>-0.9232657687920166</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3585449778806827</v>
+        <v>0.3585449778807103</v>
       </c>
     </row>
     <row r="16">
@@ -1059,16 +1059,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.140793443319634</v>
+        <v>2.140793443319625</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8037532099556847</v>
+        <v>0.8037532099556828</v>
       </c>
       <c r="D16" t="n">
-        <v>2.663495979615021</v>
+        <v>2.663495979615016</v>
       </c>
       <c r="E16" t="n">
-        <v>0.009287613265408326</v>
+        <v>0.009287613265408437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>